<commit_message>
Extra logging for authentication
</commit_message>
<xml_diff>
--- a/deploy/aws price comparison 2023-05.xlsx
+++ b/deploy/aws price comparison 2023-05.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Attack_Vector\_attack_vector2\deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44685DFD-F3A5-40DD-A22A-8F839560C37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F43DD1-6F48-44CF-B3D8-A38C0E6CBFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25395" yWindow="3075" windowWidth="21210" windowHeight="11475" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4260" yWindow="2730" windowWidth="37560" windowHeight="15885" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Application stats" sheetId="1" r:id="rId1"/>
     <sheet name="MongoDB Atlas" sheetId="3" r:id="rId2"/>
     <sheet name="App runner" sheetId="2" r:id="rId3"/>
+    <sheet name="ECS + Atlas" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="58">
   <si>
     <t>Apprunner</t>
   </si>
@@ -144,6 +145,63 @@
   </si>
   <si>
     <t>year</t>
+  </si>
+  <si>
+    <t>AWS Nat gateway</t>
+  </si>
+  <si>
+    <t>per hour</t>
+  </si>
+  <si>
+    <t>ECR</t>
+  </si>
+  <si>
+    <t>ECS</t>
+  </si>
+  <si>
+    <t>VPC</t>
+  </si>
+  <si>
+    <t>IP address</t>
+  </si>
+  <si>
+    <t>Private link</t>
+  </si>
+  <si>
+    <t>vCPU</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>total/hour</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Element</t>
+  </si>
+  <si>
+    <t>Storage GB/hour</t>
+  </si>
+  <si>
+    <t>Hour cost</t>
+  </si>
+  <si>
+    <t>Day Cost</t>
+  </si>
+  <si>
+    <t>Month cost</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Hour</t>
   </si>
 </sst>
 </file>
@@ -212,14 +270,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -732,23 +788,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60280056-7D27-4DE8-9E70-1BF0ACCE2D58}">
-  <dimension ref="A2:C27"/>
+  <dimension ref="A2:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -758,8 +815,17 @@
       <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -769,7 +835,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
@@ -781,7 +847,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -793,7 +859,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -805,7 +871,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -817,7 +883,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -828,7 +894,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
@@ -839,8 +905,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13">
@@ -848,8 +914,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="3">
@@ -857,8 +923,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>21</v>
       </c>
       <c r="B15">
@@ -869,8 +935,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>22</v>
       </c>
       <c r="B16">
@@ -882,7 +948,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="3">
@@ -959,6 +1025,242 @@
       <c r="B27" s="1">
         <f>B20+B9</f>
         <v>360.036</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C022359-425E-4296-972D-A95B889487BD}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3">
+        <f>0.1/(24*30)</f>
+        <v>1.3888888888888889E-4</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f>D3*C3</f>
+        <v>1.3888888888888889E-4</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F4" s="1">
+        <f>E3</f>
+        <v>1.3888888888888889E-4</v>
+      </c>
+      <c r="G4" s="1">
+        <f>F4*24</f>
+        <v>3.3333333333333331E-3</v>
+      </c>
+      <c r="H4" s="1">
+        <f>G4*31</f>
+        <v>0.10333333333333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <v>0.04</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f>D6*C6</f>
+        <v>0.04</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <f>D7*C7</f>
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="1">
+        <f>SUM(E6:E7)</f>
+        <v>4.8800000000000003E-2</v>
+      </c>
+      <c r="G8" s="1">
+        <f>F8*24</f>
+        <v>1.1712</v>
+      </c>
+      <c r="H8" s="1">
+        <f>G8*31</f>
+        <v>36.307200000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f>D10*C10</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <f>D11*C11</f>
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="1">
+        <f>SUM(E10:E11)</f>
+        <v>1.6E-2</v>
+      </c>
+      <c r="G12" s="1">
+        <f>F12*24</f>
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="H12" s="1">
+        <f>G12*31</f>
+        <v>11.904</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="1">
+        <f>SUM(F1:F14)</f>
+        <v>6.4938888888888893E-2</v>
+      </c>
+      <c r="G15" s="1">
+        <f>SUM(G1:G14)</f>
+        <v>1.5585333333333335</v>
+      </c>
+      <c r="H15" s="1">
+        <f>SUM(H1:H14)</f>
+        <v>48.31453333333333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Github action test: configure secrets in task definition
</commit_message>
<xml_diff>
--- a/deploy/aws price comparison 2023-05.xlsx
+++ b/deploy/aws price comparison 2023-05.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Attack_Vector\_attack_vector2\deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F43DD1-6F48-44CF-B3D8-A38C0E6CBFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD37973-CA28-4799-B142-7633C399FD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="2730" windowWidth="37560" windowHeight="15885" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6210" yWindow="4680" windowWidth="37560" windowHeight="15885" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Application stats" sheetId="1" r:id="rId1"/>
@@ -208,6 +208,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -270,12 +273,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1037,7 +1041,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,15 +1127,15 @@
       <c r="B6" t="s">
         <v>46</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>0.04</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="E6">
         <f>D6*C6</f>
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -1145,11 +1149,11 @@
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <f>D7*C7</f>
-        <v>8.8000000000000005E-3</v>
+        <v>4.4000000000000003E-3</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -1158,15 +1162,15 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F8" s="1">
         <f>SUM(E6:E7)</f>
-        <v>4.8800000000000003E-2</v>
+        <v>1.44E-2</v>
       </c>
       <c r="G8" s="1">
         <f>F8*24</f>
-        <v>1.1712</v>
+        <v>0.34560000000000002</v>
       </c>
       <c r="H8" s="1">
         <f>G8*31</f>
-        <v>36.307200000000002</v>
+        <v>10.713600000000001</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1181,7 +1185,7 @@
       <c r="B10" t="s">
         <v>44</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D10">
@@ -1199,7 +1203,7 @@
       <c r="B11" t="s">
         <v>45</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="5">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="D11">
@@ -1241,15 +1245,15 @@
       </c>
       <c r="F15" s="1">
         <f>SUM(F1:F14)</f>
-        <v>6.4938888888888893E-2</v>
+        <v>3.0538888888888886E-2</v>
       </c>
       <c r="G15" s="1">
         <f>SUM(G1:G14)</f>
-        <v>1.5585333333333335</v>
+        <v>0.73293333333333344</v>
       </c>
       <c r="H15" s="1">
         <f>SUM(H1:H14)</f>
-        <v>48.31453333333333</v>
+        <v>22.720933333333335</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>